<commit_message>
work in carddirs and charity_bag
</commit_message>
<xml_diff>
--- a/newCards.xlsx
+++ b/newCards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Stuff" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12729" uniqueCount="4544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12817" uniqueCount="4577">
   <si>
     <t>Name</t>
   </si>
@@ -13654,6 +13654,105 @@
   </si>
   <si>
     <t>161012_MBKC_080.jpg</t>
+  </si>
+  <si>
+    <t>Jimmy Foxx</t>
+  </si>
+  <si>
+    <t>Screenshot_20170211-093359.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170218-124932.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170219-171757.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170206-213235.png</t>
+  </si>
+  <si>
+    <t>Jason Hammell</t>
+  </si>
+  <si>
+    <t>IMG_20170211_175036.jpg</t>
+  </si>
+  <si>
+    <t>Screenshot_20170211-093601.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170217-203108.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170218-172712.png</t>
+  </si>
+  <si>
+    <t>John Wooden</t>
+  </si>
+  <si>
+    <t>Screenshot_20170209-223003.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170219-172028.png</t>
+  </si>
+  <si>
+    <t>Draymon Greene</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>Screenshot_20170211-092937.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170211-093734.png</t>
+  </si>
+  <si>
+    <t>Fred McGriff</t>
+  </si>
+  <si>
+    <t>Screenshot_20170209-191856.png</t>
+  </si>
+  <si>
+    <t>Christopher Eccleston</t>
+  </si>
+  <si>
+    <t>Screenshot_20170217-203004.png</t>
+  </si>
+  <si>
+    <t>Jimmy Butler</t>
+  </si>
+  <si>
+    <t>Bulls</t>
+  </si>
+  <si>
+    <t>Screenshot_20170217-203532.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170218-125115.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170209-182115.png</t>
+  </si>
+  <si>
+    <t>Screenshot_20170206-213404.png</t>
+  </si>
+  <si>
+    <t>Glenn Robinson III</t>
+  </si>
+  <si>
+    <t>Pacers</t>
+  </si>
+  <si>
+    <t>Dunk Contest</t>
+  </si>
+  <si>
+    <t>Screenshot_20170219-172238.png</t>
+  </si>
+  <si>
+    <t>Meteoric</t>
+  </si>
+  <si>
+    <t>Screenshot_20170208-194102.png</t>
   </si>
 </sst>
 </file>
@@ -14506,10 +14605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14538,6 +14637,313 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2605</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2589</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4549</v>
+      </c>
+      <c r="B7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4520</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4475</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3064</v>
+      </c>
+      <c r="B10" t="s">
+        <v>703</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2482</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2745</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4554</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4526</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4557</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4558</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4561</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2938</v>
+      </c>
+      <c r="C15" t="s">
+        <v>434</v>
+      </c>
+      <c r="D15">
+        <v>2016</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4412</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4565</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4430</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3508</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>703</v>
+      </c>
+      <c r="C19" t="s">
+        <v>434</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2570</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4571</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4572</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2530</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4573</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2825</v>
+      </c>
+      <c r="B22" t="s">
+        <v>703</v>
+      </c>
+      <c r="C22" t="s">
+        <v>434</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4575</v>
+      </c>
+      <c r="F22" t="s">
+        <v>4576</v>
       </c>
     </row>
   </sheetData>
@@ -45667,7 +46073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F890"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A829" workbookViewId="0">
+    <sheetView topLeftCell="A829" workbookViewId="0">
       <selection activeCell="A831" sqref="A831"/>
     </sheetView>
   </sheetViews>

</xml_diff>